<commit_message>
Update Lefey evidence.xlsx A1-A6
</commit_message>
<xml_diff>
--- a/Lefey/evidence.xlsx
+++ b/Lefey/evidence.xlsx
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="45">
   <si>
     <t>TeamName</t>
   </si>
@@ -96,34 +96,70 @@
     <t>ClassID</t>
   </si>
   <si>
-    <t>tx hash on irisnet</t>
+    <t>34F911E875F6EB01A37458696B8AAAD42C22B9D182E17EFD686521CC6B5807E1</t>
   </si>
   <si>
-    <t>class id you issued</t>
+    <t>lefeyGON</t>
   </si>
   <si>
     <t>NFTID</t>
   </si>
   <si>
-    <t>nft id you minted</t>
+    <t>B1B68BCF457AC050B1C2305A4CC1095A68A9ED52E62B260E880E8DA06CD6E90B</t>
+  </si>
+  <si>
+    <t>lefeyGON001</t>
+  </si>
+  <si>
+    <t>F0DC448A511857E6EA2CA07159D3AB45F84EA7CAB83D80638593112AFD1265B6</t>
+  </si>
+  <si>
+    <t>lefeyGON002</t>
+  </si>
+  <si>
+    <t>72469A2C8105B451D3617A107AA147E3E65412E7B760A98C2F93213C2CB1C043</t>
+  </si>
+  <si>
+    <t>lefeyGON003</t>
+  </si>
+  <si>
+    <t>E0E5DF4421633A3976B5713E466591BED232CA187B054466D8A68A1CD63E71FD</t>
+  </si>
+  <si>
+    <t>lefeyGON004</t>
   </si>
   <si>
     <t>ChainID</t>
   </si>
   <si>
-    <t>ibc class on dest chain</t>
+    <t>4C813FF1326D0CB3F7A5B5B559B6A77360CCBB2703185653E2A95B01B941C438</t>
+  </si>
+  <si>
+    <t>wasm.juno1kqx4e2kvgudr67ugwxk77duh3k2nsv0nrwytmlqsauedj3gafcys75nmhu</t>
+  </si>
+  <si>
+    <t>uni-6</t>
+  </si>
+  <si>
+    <t>A4FA42A8322305CA0CEA0066214D91894359C24DD734B309E8CCD6D1C5DEDC6B</t>
+  </si>
+  <si>
+    <t>ibc/E66B1DDB8C7BE439D4EE1C5250BB5B312C492587B5FA58DDC2D53F3662DDE062</t>
+  </si>
+  <si>
+    <t>uptick_7000-2</t>
+  </si>
+  <si>
+    <t>21BEF8C4FF1A3246999EF654E97CDF91B667E39D2C2AEC11D0844FD5C26DB6DC</t>
+  </si>
+  <si>
+    <t>96E9DE4F57B8DDF42D989CEC69EA22EDD5DE90F2378462AE912FD2DF66A53329</t>
+  </si>
+  <si>
+    <t>ibc class on chain</t>
   </si>
   <si>
     <t>nft id</t>
-  </si>
-  <si>
-    <t>dest chain id</t>
-  </si>
-  <si>
-    <t>tx hash on dest chain</t>
-  </si>
-  <si>
-    <t>ibc class on chain</t>
   </si>
   <si>
     <t>tx hash on that chain</t>
@@ -160,7 +196,6 @@
     <font>
       <color theme="1"/>
       <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -195,18 +230,17 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment readingOrder="0"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
+    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf borderId="1" fillId="3" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
@@ -1600,7 +1634,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -1612,11 +1645,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -2636,7 +2669,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -2648,11 +2680,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -3672,7 +3704,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -3684,11 +3715,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -4708,7 +4739,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -4720,11 +4750,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -5744,7 +5774,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -5752,25 +5781,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -6788,7 +6817,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -6796,25 +6824,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -7832,7 +7860,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -7840,25 +7867,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -8876,7 +8903,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -8884,25 +8910,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -9920,7 +9946,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -9928,25 +9953,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -10964,7 +10989,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -10972,25 +10996,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -12008,7 +12032,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="2" width="17.88"/>
-    <col customWidth="1" min="3" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -13044,7 +13067,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -13052,25 +13074,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -14088,7 +14110,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -14096,25 +14117,25 @@
         <v>16</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>28</v>
+      <c r="A2" s="6" t="s">
+        <v>40</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>29</v>
+      <c r="B2" s="6" t="s">
+        <v>41</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>30</v>
+      <c r="A3" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="5" t="s">
-        <v>30</v>
+      <c r="A4" s="6" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="5" ht="12.75" customHeight="1"/>
@@ -15140,13 +15161,13 @@
       </c>
     </row>
     <row r="2" ht="15.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
+      <c r="A3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1"/>
@@ -16177,13 +16198,13 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
+      <c r="A3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1"/>
@@ -17214,13 +17235,13 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
+      <c r="A3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1"/>
@@ -18251,13 +18272,13 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>31</v>
+      <c r="A2" s="6" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1">
-      <c r="A3" s="5" t="s">
-        <v>32</v>
+      <c r="A3" s="6" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="4" ht="12.75" customHeight="1"/>
@@ -19281,7 +19302,6 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -19297,18 +19317,48 @@
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="B2" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1"/>
-    <row r="4" ht="12.75" customHeight="1"/>
-    <row r="5" ht="12.75" customHeight="1"/>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" ht="12.75" customHeight="1">
+      <c r="A4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" ht="12.75" customHeight="1">
+      <c r="A5" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>28</v>
+      </c>
+    </row>
     <row r="6" ht="12.75" customHeight="1"/>
     <row r="7" ht="12.75" customHeight="1"/>
     <row r="8" ht="12.75" customHeight="1"/>
@@ -20324,7 +20374,6 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -20338,24 +20387,26 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
-    <row r="3" ht="12.75" customHeight="1"/>
+    <row r="3" ht="12.75" customHeight="1">
+      <c r="A3" s="5"/>
+    </row>
     <row r="4" ht="12.75" customHeight="1"/>
     <row r="5" ht="12.75" customHeight="1"/>
     <row r="6" ht="12.75" customHeight="1"/>
@@ -21373,7 +21424,6 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -21387,21 +21437,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -22422,7 +22472,6 @@
   <cols>
     <col customWidth="1" min="1" max="2" width="17.88"/>
     <col customWidth="1" min="3" max="3" width="16.0"/>
-    <col customWidth="1" min="4" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -22436,21 +22485,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -23473,7 +23522,6 @@
     <col customWidth="1" min="2" max="2" width="16.0"/>
     <col customWidth="1" min="3" max="3" width="16.25"/>
     <col customWidth="1" min="4" max="4" width="14.38"/>
-    <col customWidth="1" min="5" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -23487,21 +23535,21 @@
         <v>20</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
       <c r="A2" s="5" t="s">
-        <v>26</v>
+        <v>37</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>27</v>
+        <v>34</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>24</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -24521,7 +24569,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -24533,11 +24580,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>
@@ -25557,7 +25604,6 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.0"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="16.0"/>
-    <col customWidth="1" min="2" max="6" width="12.63"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" customHeight="1">
@@ -25569,11 +25615,11 @@
       </c>
     </row>
     <row r="2" ht="12.75" customHeight="1">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
+      <c r="A2" s="6" t="s">
+        <v>38</v>
       </c>
-      <c r="B2" s="5" t="s">
-        <v>24</v>
+      <c r="B2" s="6" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" ht="12.75" customHeight="1"/>

</xml_diff>